<commit_message>
MVC UPDATE STS GENAP 2024
</commit_message>
<xml_diff>
--- a/temp_doc/DATA KELAS FIX.xlsx
+++ b/temp_doc/DATA KELAS FIX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2ABC70-D86D-7E4F-9EAC-49654073EE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6E253D-6892-E145-9BA4-E901C9A15C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -61,12 +61,6 @@
     <t>XI AKL 2</t>
   </si>
   <si>
-    <t>XII AKL 1</t>
-  </si>
-  <si>
-    <t>XII AKL 2</t>
-  </si>
-  <si>
     <t>DKV</t>
   </si>
   <si>
@@ -88,12 +82,6 @@
     <t>XI MPLB 2</t>
   </si>
   <si>
-    <t>XII MPLB 1</t>
-  </si>
-  <si>
-    <t>XII MPLB 2</t>
-  </si>
-  <si>
     <t>TJKT</t>
   </si>
   <si>
@@ -115,15 +103,6 @@
     <t>XI TJKT 3</t>
   </si>
   <si>
-    <t>XII TJKT 1</t>
-  </si>
-  <si>
-    <t>XII TJKT 2</t>
-  </si>
-  <si>
-    <t>XII TJKT 3</t>
-  </si>
-  <si>
     <t>X DKV</t>
   </si>
   <si>
@@ -134,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">XI PM </t>
-  </si>
-  <si>
-    <t>XII PM</t>
   </si>
 </sst>
 </file>
@@ -207,9 +183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -353,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -495,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,7 +482,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:C27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,10 +525,10 @@
         <v>1029404</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -560,10 +536,10 @@
         <v>1030404</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -571,10 +547,10 @@
         <v>1031404</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -582,10 +558,10 @@
         <v>1032404</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -593,10 +569,10 @@
         <v>1033404</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -604,10 +580,10 @@
         <v>1034404</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -615,10 +591,10 @@
         <v>1035404</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -648,10 +624,10 @@
         <v>1038404</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -659,10 +635,10 @@
         <v>1039404</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -670,10 +646,10 @@
         <v>1040404</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,10 +657,10 @@
         <v>1041404</v>
       </c>
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -692,10 +668,10 @@
         <v>1042404</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,10 +679,10 @@
         <v>1043404</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,99 +690,35 @@
         <v>1044404</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1045404</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1046404</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>1047404</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1048404</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1049404</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1050404</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1051404</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1052404</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C28" s="2"/>

</xml_diff>